<commit_message>
create print dict method
</commit_message>
<xml_diff>
--- a/bench/results.xlsx
+++ b/bench/results.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Workspace/ACI/xiang/edge-computing-models/bench/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4FABAD-646A-C747-86BB-CBEB58361B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2120" yWindow="880" windowWidth="31900" windowHeight="22740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
   <si>
     <t>Small Size - OCR [100 KBs Input]</t>
   </si>
@@ -65,13 +71,19 @@
   </si>
   <si>
     <t>Large Size - Smith-Waterman [100 KBs Input]</t>
+  </si>
+  <si>
+    <t>75 Iterations (25 Each)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +120,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +172,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -186,6 +206,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -220,9 +241,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -395,19 +417,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -424,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -435,21 +464,21 @@
         <v>10.6739</v>
       </c>
       <c r="D3">
-        <v>0.0362</v>
+        <v>3.6200000000000003E-2</v>
       </c>
       <c r="E3">
-        <v>10.7101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>10.710100000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>34.8822</v>
+        <v>34.882199999999997</v>
       </c>
       <c r="D4">
         <v>0.1895</v>
@@ -458,7 +487,7 @@
         <v>35.0717</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -466,21 +495,21 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>70.7723</v>
+        <v>70.772300000000001</v>
       </c>
       <c r="D5">
-        <v>0.0497</v>
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>70.822</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>70.822000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -497,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -505,33 +534,33 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>5.2869</v>
+        <v>5.2869000000000002</v>
       </c>
       <c r="D9">
-        <v>0.0741</v>
+        <v>7.4099999999999999E-2</v>
       </c>
       <c r="E9">
-        <v>5.361</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>5.3609999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>29.7432</v>
+        <v>29.743200000000002</v>
       </c>
       <c r="D10">
-        <v>0.2562</v>
+        <v>0.25619999999999998</v>
       </c>
       <c r="E10">
-        <v>29.9994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>29.999400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -539,21 +568,21 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>77.59990000000001</v>
+        <v>77.599900000000005</v>
       </c>
       <c r="D11">
-        <v>0.0258</v>
+        <v>2.58E-2</v>
       </c>
       <c r="E11">
-        <v>77.62570000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>77.625700000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -570,7 +599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -578,18 +607,18 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>6.0341</v>
+        <v>6.0340999999999996</v>
       </c>
       <c r="D15">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E15">
-        <v>6.0851</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>6.0850999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -598,13 +627,13 @@
         <v>36.7821</v>
       </c>
       <c r="D16">
-        <v>0.2696</v>
+        <v>0.26960000000000001</v>
       </c>
       <c r="E16">
-        <v>37.0517</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>37.051699999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -612,21 +641,21 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>99.34820000000001</v>
+        <v>99.348200000000006</v>
       </c>
       <c r="D17">
-        <v>0.0231</v>
+        <v>2.3099999999999999E-2</v>
       </c>
       <c r="E17">
-        <v>99.37130000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>99.371300000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -643,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -651,18 +680,18 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>17.1651</v>
+        <v>17.165099999999999</v>
       </c>
       <c r="D21">
-        <v>0.1543</v>
+        <v>0.15429999999999999</v>
       </c>
       <c r="E21">
-        <v>17.3194</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>17.319400000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -671,13 +700,13 @@
         <v>99.8172</v>
       </c>
       <c r="D22">
-        <v>0.5227000000000001</v>
+        <v>0.52270000000000005</v>
       </c>
       <c r="E22">
         <v>100.3399</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -685,21 +714,21 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>264.7352</v>
+        <v>264.73520000000002</v>
       </c>
       <c r="D23">
-        <v>0.0265</v>
+        <v>2.6499999999999999E-2</v>
       </c>
       <c r="E23">
-        <v>264.7617</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>264.76170000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -716,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -724,18 +753,18 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>18.5464</v>
+        <v>18.546399999999998</v>
       </c>
       <c r="D27">
-        <v>0.0741</v>
+        <v>7.4099999999999999E-2</v>
       </c>
       <c r="E27">
         <v>18.6205</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -744,13 +773,13 @@
         <v>117.1889</v>
       </c>
       <c r="D28">
-        <v>0.275</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E28">
         <v>117.4639</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -758,21 +787,21 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>314.7858</v>
+        <v>314.78579999999999</v>
       </c>
       <c r="D29">
-        <v>0.024</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E29">
         <v>314.8098</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -789,7 +818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -797,33 +826,36 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <v>87.4087</v>
+        <v>87.408699999999996</v>
       </c>
       <c r="D33">
-        <v>0.0842</v>
+        <v>8.4199999999999997E-2</v>
       </c>
       <c r="E33">
-        <v>87.49289999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>87.492899999999992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34">
-        <v>227.6826</v>
+        <v>227.68260000000001</v>
       </c>
       <c r="D34">
-        <v>0.2861</v>
+        <v>0.28610000000000002</v>
       </c>
       <c r="E34">
-        <v>227.9687</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>227.96870000000001</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -834,18 +866,18 @@
         <v>447.2824</v>
       </c>
       <c r="D35">
-        <v>0.0588</v>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="E35">
-        <v>447.3412</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>447.34120000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -862,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -870,33 +902,33 @@
         <v>7</v>
       </c>
       <c r="C39">
-        <v>86.07769999999999</v>
+        <v>86.077699999999993</v>
       </c>
       <c r="D39">
-        <v>0.5098</v>
+        <v>0.50980000000000003</v>
       </c>
       <c r="E39">
-        <v>86.58749999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>86.587499999999991</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40">
-        <v>501.7732</v>
+        <v>501.77319999999997</v>
       </c>
       <c r="D40">
-        <v>2.0292</v>
+        <v>2.0291999999999999</v>
       </c>
       <c r="E40">
-        <v>503.8024</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>503.80239999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -904,21 +936,21 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>1321.773</v>
+        <v>1321.7729999999999</v>
       </c>
       <c r="D41">
-        <v>0.0248</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="E41">
-        <v>1321.7978</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>1321.7978000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -935,7 +967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -943,33 +975,33 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>51.4267</v>
+        <v>51.426699999999997</v>
       </c>
       <c r="D45">
         <v>0.1115</v>
       </c>
       <c r="E45">
-        <v>51.5382</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>51.538200000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46">
-        <v>307.9444</v>
+        <v>307.94439999999997</v>
       </c>
       <c r="D46">
-        <v>0.2861</v>
+        <v>0.28610000000000002</v>
       </c>
       <c r="E46">
-        <v>308.2304999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>308.23049999999989</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -980,10 +1012,10 @@
         <v>853.5634</v>
       </c>
       <c r="D47">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="E47">
-        <v>853.5904</v>
+        <v>853.59040000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tqmd to iot client running process
</commit_message>
<xml_diff>
--- a/bench/results.xlsx
+++ b/bench/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Workspace/ACI/xiang/edge-computing-models/bench/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BC28CA-3857-D04F-A581-5C4541DA7552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA89362-D775-EA40-8207-1FEE50180A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="880" windowWidth="31700" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="880" windowWidth="29040" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
-  <si>
-    <t>OCR - Small Size [100 KBs Input]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+  <si>
+    <t>OCR - Small Size [11KB Input]</t>
   </si>
   <si>
     <t>Iteration</t>
@@ -40,19 +40,40 @@
     <t>Total Finishing Time (Sec)</t>
   </si>
   <si>
+    <t>25 Iterations</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>IoT Device</t>
+  </si>
+  <si>
+    <t>OCR - Medium Size [500KB Input]</t>
+  </si>
+  <si>
+    <t>OCR - Large Size [1.5MB Input]</t>
+  </si>
+  <si>
+    <t>Sentiment Analysis - Small Size [60 Reviews Input]</t>
+  </si>
+  <si>
     <t>54 Iterations</t>
   </si>
   <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>Edge</t>
-  </si>
-  <si>
-    <t>OCR - Medium Size [500 KBs Input]</t>
-  </si>
-  <si>
-    <t>OCR - Large Size [1000 KBs Input]</t>
+    <t>Sentiment Analysis - Medium Size [200 Reviews Input]</t>
+  </si>
+  <si>
+    <t>Sentiment Analysis - Large Size [1000 Reviews Input]</t>
+  </si>
+  <si>
+    <t>Smith-Waterman - Small Size [25 KBs Input]</t>
+  </si>
+  <si>
+    <t>Smith-Waterman - Medium Size [50 KBs Input]</t>
+  </si>
+  <si>
+    <t>Smith-Waterman - Large Size [100 KBs Input]</t>
   </si>
 </sst>
 </file>
@@ -394,20 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -439,13 +453,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29.2148</v>
+        <v>6.5442999999999998</v>
       </c>
       <c r="D3">
-        <v>8.9599999999999999E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E3">
-        <v>29.304400000000001</v>
+        <v>6.6313000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -456,13 +470,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>25.214600000000001</v>
+        <v>5.8672000000000004</v>
       </c>
       <c r="D4">
-        <v>5.57E-2</v>
+        <v>7.9100000000000004E-2</v>
       </c>
       <c r="E4">
-        <v>25.270299999999999</v>
+        <v>5.9463000000000008</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -495,13 +509,13 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>172.5685</v>
+        <v>128.2758</v>
       </c>
       <c r="D8">
-        <v>0.1038</v>
+        <v>9.1700000000000004E-2</v>
       </c>
       <c r="E8">
-        <v>172.67230000000001</v>
+        <v>128.36750000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -512,13 +526,13 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>144.58699999999999</v>
+        <v>406.92349999999999</v>
       </c>
       <c r="D9">
-        <v>9.6100000000000005E-2</v>
+        <v>9.1200000000000003E-2</v>
       </c>
       <c r="E9">
-        <v>144.6831</v>
+        <v>407.0147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -551,13 +565,13 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>213.04069999999999</v>
+        <v>188.6251</v>
       </c>
       <c r="D13">
-        <v>0.1237</v>
+        <v>0.1666</v>
       </c>
       <c r="E13">
-        <v>213.1644</v>
+        <v>188.79169999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -568,13 +582,349 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>165.75129999999999</v>
+        <v>410.55709999999999</v>
       </c>
       <c r="D14">
-        <v>0.12039999999999999</v>
+        <v>9.2700000000000005E-2</v>
       </c>
       <c r="E14">
-        <v>165.8717</v>
+        <v>410.64980000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>23.1357</v>
+      </c>
+      <c r="D18">
+        <v>0.16550000000000001</v>
+      </c>
+      <c r="E18">
+        <v>23.301200000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>152.7544</v>
+      </c>
+      <c r="D19">
+        <v>5.2200000000000003E-2</v>
+      </c>
+      <c r="E19">
+        <v>152.8066</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>40.601799999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E23">
+        <v>40.897799999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>565.69989999999996</v>
+      </c>
+      <c r="D24">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="E24">
+        <v>565.75379999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>371.71019999999999</v>
+      </c>
+      <c r="D28">
+        <v>1.1002000000000001</v>
+      </c>
+      <c r="E28">
+        <v>372.81040000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>2802.701</v>
+      </c>
+      <c r="D29">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="E29">
+        <v>2802.7573000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>26.1891</v>
+      </c>
+      <c r="D33">
+        <v>0.14530000000000001</v>
+      </c>
+      <c r="E33">
+        <v>26.334399999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>195.66200000000001</v>
+      </c>
+      <c r="D34">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="E34">
+        <v>195.71860000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>156.00360000000001</v>
+      </c>
+      <c r="D38">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="E38">
+        <v>156.16470000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>678.99109999999996</v>
+      </c>
+      <c r="D39">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="E39">
+        <v>679.04919999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>239.92670000000001</v>
+      </c>
+      <c r="D43">
+        <v>0.214</v>
+      </c>
+      <c r="E43">
+        <v>240.14070000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>1881.4924000000001</v>
+      </c>
+      <c r="D44">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="E44">
+        <v>1881.5526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>